<commit_message>
terminei o cadastro de novo usuario e coloque um print para capturar a utima tela
</commit_message>
<xml_diff>
--- a/src/main/java/arquivos/bancoDados.xlsx
+++ b/src/main/java/arquivos/bancoDados.xlsx
@@ -3,12 +3,12 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\saulo.silva\eclipse-workspace\tdd\src\main\java\arquivos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2F78CC2-E966-4F05-A7B4-47776D04DACA}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08160ECA-BB1A-482D-B477-736BF8720890}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{D514BC7B-BE3F-4BB9-9548-BB59BDF80586}"/>
   </bookViews>
@@ -17,7 +17,7 @@
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="36">
   <si>
     <t>Usuario</t>
   </si>
@@ -69,9 +69,6 @@
     <t>CodigoPostal</t>
   </si>
   <si>
-    <t>saulosjs</t>
-  </si>
-  <si>
     <t>saulo.silva@rsinet.com.br</t>
   </si>
   <si>
@@ -84,9 +81,6 @@
     <t>José da Silva</t>
   </si>
   <si>
-    <t>Brasil</t>
-  </si>
-  <si>
     <t>São paulo</t>
   </si>
   <si>
@@ -99,16 +93,59 @@
     <t>Resutado</t>
   </si>
   <si>
-    <t>"921316555"</t>
-  </si>
-  <si>
-    <t>"123456789"</t>
+    <t>(11)921316555</t>
+  </si>
+  <si>
+    <t>mano</t>
+  </si>
+  <si>
+    <t>saulojosilva@hotmail.com</t>
+  </si>
+  <si>
+    <t>eita</t>
+  </si>
+  <si>
+    <t>Marcos</t>
+  </si>
+  <si>
+    <t>rapaz</t>
+  </si>
+  <si>
+    <t>Silva</t>
+  </si>
+  <si>
+    <t>(11)954423458</t>
+  </si>
+  <si>
+    <t>Algeria</t>
+  </si>
+  <si>
+    <t>Brazil</t>
+  </si>
+  <si>
+    <t>paris</t>
+  </si>
+  <si>
+    <t>rua mundi</t>
+  </si>
+  <si>
+    <t>af</t>
+  </si>
+  <si>
+    <t>(11)12345</t>
+  </si>
+  <si>
+    <t>Pass</t>
+  </si>
+  <si>
+    <t>saulosjss33</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="0"/>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -469,20 +506,20 @@
   <dimension ref="A1:M10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L2" sqref="L2"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="7.36328125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="22.7265625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.453125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.453125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.36328125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="9.6328125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="11.54296875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="7.36328125" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="22.7265625" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="9.453125" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="14.453125" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="13.0" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="11.36328125" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="15.0" collapsed="true"/>
+    <col min="10" max="10" bestFit="true" customWidth="true" width="9.6328125" collapsed="true"/>
+    <col min="12" max="12" bestFit="true" customWidth="true" width="13.1796875" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.35">
@@ -523,45 +560,86 @@
         <v>11</v>
       </c>
       <c r="M1" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
+        <v>35</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="C2" t="s">
         <v>13</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E2" t="s">
         <v>14</v>
       </c>
-      <c r="D2" t="s">
-        <v>14</v>
-      </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
         <v>15</v>
       </c>
-      <c r="F2" t="s">
+      <c r="G2" t="s">
+        <v>20</v>
+      </c>
+      <c r="H2" t="s">
+        <v>29</v>
+      </c>
+      <c r="I2" t="s">
         <v>16</v>
       </c>
-      <c r="G2" t="s">
+      <c r="J2" t="s">
+        <v>17</v>
+      </c>
+      <c r="K2" t="s">
+        <v>18</v>
+      </c>
+      <c r="L2" t="s">
+        <v>33</v>
+      </c>
+      <c r="M2" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>25</v>
+      </c>
+      <c r="B3" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="H2" t="s">
-        <v>17</v>
-      </c>
-      <c r="I2" t="s">
-        <v>18</v>
-      </c>
-      <c r="J2" t="s">
-        <v>19</v>
-      </c>
-      <c r="K2" t="s">
-        <v>20</v>
-      </c>
-      <c r="L2" t="s">
+      <c r="C3" t="s">
+        <v>21</v>
+      </c>
+      <c r="D3" t="s">
         <v>23</v>
+      </c>
+      <c r="E3" t="s">
+        <v>24</v>
+      </c>
+      <c r="F3" t="s">
+        <v>26</v>
+      </c>
+      <c r="G3" t="s">
+        <v>27</v>
+      </c>
+      <c r="H3" t="s">
+        <v>28</v>
+      </c>
+      <c r="I3" t="s">
+        <v>30</v>
+      </c>
+      <c r="J3" t="s">
+        <v>31</v>
+      </c>
+      <c r="K3" t="s">
+        <v>32</v>
+      </c>
+      <c r="L3" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.35">
@@ -570,8 +648,9 @@
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B2" r:id="rId1" xr:uid="{7080927B-4433-4CAC-BB96-EF975263CE62}"/>
+    <hyperlink ref="B3" r:id="rId2" xr:uid="{037C12C2-9D84-4A44-A716-0B9C3859C82A}"/>
   </hyperlinks>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId3"/>
 </worksheet>
 </file>
</xml_diff>